<commit_message>
Add missing Japanese translation
</commit_message>
<xml_diff>
--- a/Config/JA/Checklist.xlsx
+++ b/Config/JA/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABD9B5F-02CA-4C21-A008-39E7CCD679DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C614EE6-F852-4E02-B11B-099157AAA95F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="174">
   <si>
     <t>最上位階層のアクティビティ（基本的にFlowchartやSequence）には、ワークフローの目的・概要を簡潔に注釈することを推奨します。これにより、開発者はワークフローの目的・インプット・アウトプット・前提条件を素早く把握することができます。</t>
     <rPh sb="0" eb="3">
@@ -1662,10 +1662,6 @@
   </si>
   <si>
     <t>必ず含まれてなければならない必須ファイルがCoEにより定義されていることがあります。このチェックは、引数で定義された必須ファイルが含まれているかどうか確認します。</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>プロジェクトフォルダに必須ファイルを追加してください。</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -1746,16 +1742,7 @@
     <t>無許可のアクティビティ</t>
   </si>
   <si>
-    <t>Missing project entry point workflow</t>
-  </si>
-  <si>
     <t>Checks\Standard\MissingProjectEntryPointWorkflow.xaml</t>
-  </si>
-  <si>
-    <t>The project.json configuration file defines a workflow (usually Main.xaml) to act as the entry point for the project and this workflow should be included in the project.</t>
-  </si>
-  <si>
-    <t>Make sure the project contains the entry point workflow as defined in project.json.</t>
   </si>
   <si>
     <t>無許可のアプリケーション</t>
@@ -1863,6 +1850,19 @@
   </si>
   <si>
     <t>CoE（Centre of Excellence)のセキュリティ対策によって、ロボットはメールを送信することが禁止されています。人が確認できるようにメッセージを下書きとして保存してください。</t>
+  </si>
+  <si>
+    <t>プロジェクトエントリポイントワークフローの欠損</t>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">ケッソン </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>project.json設定ファイルには、プロジェクトのエントリーポイントとして動作するワークフロー（通常はMain.xaml）を定義します。このワークフローをプロジェクトに含める必要があります。</t>
+  </si>
+  <si>
+    <t>プロジェクトに、project.jsonで定義されているエントリポイントワークフローが含まれていることを確認します。</t>
   </si>
 </sst>
 </file>
@@ -2332,7 +2332,7 @@
     <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.36328125" style="1" customWidth="1"/>
     <col min="4" max="5" width="28.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="49.90625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49.81640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="39.6328125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.6328125" style="1"/>
   </cols>
@@ -2362,7 +2362,7 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="72.5">
       <c r="A2" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="72.5">
       <c r="A3" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="87">
       <c r="A4" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
@@ -2425,7 +2425,7 @@
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="116">
       <c r="A5" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
@@ -2446,7 +2446,7 @@
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="101.5">
       <c r="A6" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>12</v>
@@ -2455,7 +2455,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>50</v>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" ht="101.5">
       <c r="A7" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>13</v>
@@ -2478,7 +2478,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>50</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="159.5">
       <c r="A8" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>28</v>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" ht="159.5">
       <c r="A9" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>31</v>
@@ -2534,7 +2534,7 @@
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" ht="159.5">
       <c r="A10" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>19</v>
@@ -2549,7 +2549,7 @@
         <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>18</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="11" spans="1:7" ht="159.5">
       <c r="A11" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>20</v>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="12" spans="1:7" ht="101.5">
       <c r="A12" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>34</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="13" spans="1:7" ht="116">
       <c r="A13" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>55</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="14" spans="1:7" ht="130.5">
       <c r="A14" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>61</v>
@@ -2643,7 +2643,7 @@
     </row>
     <row r="15" spans="1:7" ht="130.5">
       <c r="A15" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>64</v>
@@ -2664,7 +2664,7 @@
     </row>
     <row r="16" spans="1:7" ht="159.5">
       <c r="A16" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>67</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="17" spans="1:7" ht="130.5">
       <c r="A17" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>58</v>
@@ -2708,7 +2708,7 @@
     </row>
     <row r="18" spans="1:7" ht="87">
       <c r="A18" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>73</v>
@@ -2729,7 +2729,7 @@
     </row>
     <row r="19" spans="1:7" s="13" customFormat="1" ht="116">
       <c r="A19" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>105</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="87">
       <c r="A20" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>108</v>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="21" spans="1:7" s="13" customFormat="1" ht="58">
       <c r="A21" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>111</v>
@@ -2792,13 +2792,13 @@
     </row>
     <row r="22" spans="1:7" ht="58">
       <c r="A22" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
@@ -2813,13 +2813,13 @@
     </row>
     <row r="23" spans="1:7" ht="58">
       <c r="A23" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
@@ -2834,13 +2834,13 @@
     </row>
     <row r="24" spans="1:7" ht="43.5">
       <c r="A24" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
@@ -2855,98 +2855,98 @@
     </row>
     <row r="25" spans="1:7" ht="72.5">
       <c r="A25" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>127</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>128</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F25" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" s="12" t="s">
         <v>130</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="217.5">
       <c r="A26" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C26" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F26" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="130.5">
       <c r="A27" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>147</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="72.5">
       <c r="A28" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="3" customFormat="1" ht="58">
       <c r="A29" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>102</v>
@@ -2958,119 +2958,119 @@
         <v>50</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="13" customFormat="1" ht="58">
       <c r="A30" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="13" customFormat="1" ht="87">
       <c r="A31" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="13" customFormat="1" ht="58">
       <c r="A32" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="13" customFormat="1" ht="87">
       <c r="A33" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="13" customFormat="1" ht="72.5">
       <c r="A34" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="11" t="s">
         <v>54</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3099,14 +3099,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="8.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.90625" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
     <col min="3" max="3" width="19.36328125" customWidth="1"/>
     <col min="4" max="5" width="28.36328125" customWidth="1"/>
-    <col min="6" max="6" width="49.90625" customWidth="1"/>
-    <col min="7" max="7" width="40.08984375" customWidth="1"/>
+    <col min="6" max="6" width="49.81640625" customWidth="1"/>
+    <col min="7" max="7" width="40.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
@@ -3134,7 +3134,7 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="87">
       <c r="A2" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>25</v>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="58">
       <c r="A3" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>70</v>
@@ -3176,28 +3176,28 @@
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="58">
       <c r="A4" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="11" t="s">
         <v>54</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="203">
       <c r="A5" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>114</v>
@@ -3214,9 +3214,7 @@
       <c r="F5" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>116</v>
-      </c>
+      <c r="G5" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>

</xml_diff>

<commit_message>
Fix regression bug caused by previous optimization
</commit_message>
<xml_diff>
--- a/Config/JA/Checklist.xlsx
+++ b/Config/JA/Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C614EE6-F852-4E02-B11B-099157AAA95F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9749AB4-9C97-4BD6-9BFB-BD86B69F000F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="172">
   <si>
     <t>最上位階層のアクティビティ（基本的にFlowchartやSequence）には、ワークフローの目的・概要を簡潔に注釈することを推奨します。これにより、開発者はワークフローの目的・インプット・アウトプット・前提条件を素早く把握することができます。</t>
     <rPh sb="0" eb="3">
@@ -1694,16 +1694,8 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Yes</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>Checks\Custom\LogBrowserURL.xaml</t>
     <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Yes</t>
@@ -2331,7 +2323,8 @@
     <col min="1" max="1" width="8.6328125" style="1"/>
     <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.36328125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="28.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" style="1" customWidth="1"/>
     <col min="6" max="6" width="49.81640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="39.6328125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.6328125" style="1"/>
@@ -2362,7 +2355,7 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="72.5">
       <c r="A2" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
@@ -2383,7 +2376,7 @@
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="72.5">
       <c r="A3" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
@@ -2404,7 +2397,7 @@
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="87">
       <c r="A4" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
@@ -2425,7 +2418,7 @@
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="116">
       <c r="A5" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
@@ -2446,7 +2439,7 @@
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="101.5">
       <c r="A6" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>12</v>
@@ -2455,7 +2448,7 @@
         <v>80</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>50</v>
@@ -2469,7 +2462,7 @@
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" ht="101.5">
       <c r="A7" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>13</v>
@@ -2478,7 +2471,7 @@
         <v>81</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>50</v>
@@ -2492,7 +2485,7 @@
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="159.5">
       <c r="A8" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>28</v>
@@ -2513,7 +2506,7 @@
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" ht="159.5">
       <c r="A9" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>31</v>
@@ -2534,7 +2527,7 @@
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" ht="159.5">
       <c r="A10" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>19</v>
@@ -2549,7 +2542,7 @@
         <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>18</v>
@@ -2557,7 +2550,7 @@
     </row>
     <row r="11" spans="1:7" ht="159.5">
       <c r="A11" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>20</v>
@@ -2578,7 +2571,7 @@
     </row>
     <row r="12" spans="1:7" ht="101.5">
       <c r="A12" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>34</v>
@@ -2599,7 +2592,7 @@
     </row>
     <row r="13" spans="1:7" ht="116">
       <c r="A13" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>55</v>
@@ -2622,7 +2615,7 @@
     </row>
     <row r="14" spans="1:7" ht="130.5">
       <c r="A14" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>61</v>
@@ -2643,7 +2636,7 @@
     </row>
     <row r="15" spans="1:7" ht="130.5">
       <c r="A15" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>64</v>
@@ -2664,7 +2657,7 @@
     </row>
     <row r="16" spans="1:7" ht="159.5">
       <c r="A16" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>67</v>
@@ -2687,7 +2680,7 @@
     </row>
     <row r="17" spans="1:7" ht="130.5">
       <c r="A17" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>58</v>
@@ -2708,7 +2701,7 @@
     </row>
     <row r="18" spans="1:7" ht="87">
       <c r="A18" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>73</v>
@@ -2729,7 +2722,7 @@
     </row>
     <row r="19" spans="1:7" s="13" customFormat="1" ht="116">
       <c r="A19" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>105</v>
@@ -2750,7 +2743,7 @@
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="87">
       <c r="A20" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>108</v>
@@ -2771,7 +2764,7 @@
     </row>
     <row r="21" spans="1:7" s="13" customFormat="1" ht="58">
       <c r="A21" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>111</v>
@@ -2792,7 +2785,7 @@
     </row>
     <row r="22" spans="1:7" ht="58">
       <c r="A22" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>35</v>
@@ -2813,7 +2806,7 @@
     </row>
     <row r="23" spans="1:7" ht="58">
       <c r="A23" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>39</v>
@@ -2834,7 +2827,7 @@
     </row>
     <row r="24" spans="1:7" ht="43.5">
       <c r="A24" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>40</v>
@@ -2855,31 +2848,31 @@
     </row>
     <row r="25" spans="1:7" ht="72.5">
       <c r="A25" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>128</v>
-      </c>
       <c r="C25" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="217.5">
       <c r="A26" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>120</v>
@@ -2891,10 +2884,10 @@
         <v>50</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="130.5">
@@ -2902,22 +2895,22 @@
         <v>119</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="72.5">
@@ -2925,20 +2918,20 @@
         <v>122</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="3" customFormat="1" ht="58">
@@ -2946,7 +2939,7 @@
         <v>122</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>102</v>
@@ -2958,10 +2951,10 @@
         <v>50</v>
       </c>
       <c r="F29" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="13" customFormat="1" ht="58">
@@ -2969,22 +2962,22 @@
         <v>119</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>149</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="13" customFormat="1" ht="87">
@@ -2992,20 +2985,20 @@
         <v>119</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="13" customFormat="1" ht="58">
@@ -3013,20 +3006,20 @@
         <v>119</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="13" customFormat="1" ht="87">
@@ -3034,22 +3027,22 @@
         <v>119</v>
       </c>
       <c r="B33" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>162</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>164</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="13" customFormat="1" ht="72.5">
@@ -3057,20 +3050,20 @@
         <v>119</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="11" t="s">
         <v>54</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3104,7 +3097,8 @@
     <col min="1" max="1" width="8.6328125" customWidth="1"/>
     <col min="2" max="2" width="15.81640625" customWidth="1"/>
     <col min="3" max="3" width="19.36328125" customWidth="1"/>
-    <col min="4" max="5" width="28.36328125" customWidth="1"/>
+    <col min="4" max="4" width="28.36328125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
     <col min="6" max="6" width="49.81640625" customWidth="1"/>
     <col min="7" max="7" width="40.1796875" customWidth="1"/>
   </cols>
@@ -3134,7 +3128,7 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="87">
       <c r="A2" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>25</v>
@@ -3155,7 +3149,7 @@
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="58">
       <c r="A3" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>70</v>
@@ -3176,23 +3170,23 @@
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="58">
       <c r="A4" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="11" t="s">
         <v>54</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="203">

</xml_diff>